<commit_message>
fixing wrong component in BOM
</commit_message>
<xml_diff>
--- a/025/BOM/jlcpcb-bom.xlsx
+++ b/025/BOM/jlcpcb-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\kicad\other\esp32-light-controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\git\SDB\025\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CAA07F9D-44CC-4644-A685-D6CC3C0217F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C71EA-EF87-4F9B-B4E9-FE4D346424D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="2295" windowWidth="24675" windowHeight="15795"/>
+    <workbookView xWindow="-28740" yWindow="795" windowWidth="24675" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jlcpcb-bom" sheetId="2" r:id="rId1"/>
@@ -23,15 +23,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Abfrage - esp32-light-controller" description="Verbindung mit der Abfrage 'esp32-light-controller' in der Arbeitsmappe." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Abfrage - esp32-light-controller" description="Verbindung mit der Abfrage 'esp32-light-controller' in der Arbeitsmappe." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=esp32-light-controller;Extended Properties=&quot;&quot;" command="SELECT * FROM [esp32-light-controller]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="127">
   <si>
     <t>Column1</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Package_SO:SOIC-16_3.9x9.9mm_P1.27mm</t>
   </si>
   <si>
-    <t>C14267</t>
-  </si>
-  <si>
     <t>LM317_TO-252</t>
   </si>
   <si>
@@ -412,12 +409,15 @@
   </si>
   <si>
     <t>C10487</t>
+  </si>
+  <si>
+    <t>C84681</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -993,7 +993,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExterneDaten_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -1006,13 +1006,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="esp32_light_controller" displayName="esp32_light_controller" ref="A1:D38" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="esp32_light_controller" displayName="esp32_light_controller" ref="A1:D38" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1314,11 +1314,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,7 +1396,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,7 +1410,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1446,13 +1446,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1460,13 +1460,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,7 +1634,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,7 +1662,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,7 +1676,7 @@
         <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>70</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,7 +1704,7 @@
         <v>70</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>70</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
         <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1760,7 +1760,7 @@
         <v>83</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,32 +1774,32 @@
         <v>86</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
@@ -1821,13 +1821,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
@@ -1835,30 +1835,30 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>